<commit_message>
ajustar tela de importação erro entrando apenas na validaçao de departamentos não existe
</commit_message>
<xml_diff>
--- a/departamentos.xlsx
+++ b/departamentos.xlsx
@@ -15,7 +15,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
   <si>
     <t>E-commerce</t>
   </si>
@@ -456,7 +462,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,275 +471,283 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
         <v>36</v>
       </c>
-      <c r="B34" t="s">
-        <v>33</v>
+      <c r="B35" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>